<commit_message>
update 2a class diagram
</commit_message>
<xml_diff>
--- a/iis.xlsx
+++ b/iis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Carlo Moisés Onassis Salgado Organista</t>
   </si>
@@ -127,13 +127,16 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>Parcial 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +148,22 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,14 +183,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,24 +529,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="38.83203125" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="7" width="3.5" customWidth="1"/>
     <col min="8" max="8" width="3.83203125" customWidth="1"/>
     <col min="9" max="9" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="F1" t="s">
         <v>26</v>
       </c>
@@ -534,8 +562,11 @@
       <c r="J1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="F2">
         <v>32</v>
       </c>
@@ -552,7 +583,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -568,11 +599,23 @@
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -592,7 +635,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -612,7 +655,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -629,7 +672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -645,8 +688,11 @@
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -663,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -680,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -699,6 +745,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add w14, simpson rule
</commit_message>
<xml_diff>
--- a/iis.xlsx
+++ b/iis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="20" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -581,21 +581,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="34.5" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" customWidth="1"/>
     <col min="8" max="10" width="5.5" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="2.5" customWidth="1"/>
     <col min="13" max="13" width="5.83203125" customWidth="1"/>
     <col min="14" max="14" width="7.83203125" customWidth="1"/>
+    <col min="15" max="15" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>